<commit_message>
cleaned up VLF dated data.  Ensured that 1's and 0's were placed correctly.  Amended code to consistently graph correctly and so that it could be run multiple times.
</commit_message>
<xml_diff>
--- a/vuf_final_all.xlsx
+++ b/vuf_final_all.xlsx
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FE90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ER59" workbookViewId="0">
-      <selection activeCell="FC90" sqref="FC90"/>
+    <sheetView tabSelected="1" topLeftCell="EO1" workbookViewId="0">
+      <selection activeCell="FF1" sqref="FF1:FF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -43336,7 +43336,7 @@
         <v>21</v>
       </c>
       <c r="BT88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU88">
         <v>55</v>
@@ -44031,7 +44031,7 @@
         <v>16</v>
       </c>
       <c r="EL89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EM89">
         <v>1</v>
@@ -44516,7 +44516,7 @@
         <v>27</v>
       </c>
       <c r="EL90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EM90">
         <v>1</v>

</xml_diff>